<commit_message>
Validate if url is accessible or not
</commit_message>
<xml_diff>
--- a/src/main/resources/9.30.processed.xlsx
+++ b/src/main/resources/9.30.processed.xlsx
@@ -304,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,6 +315,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkGrid">
+        <bgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
@@ -437,8 +447,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Excel Built-in Normal" xfId="3"/>

</xml_diff>